<commit_message>
corregida gramatica del informe
</commit_message>
<xml_diff>
--- a/Documentos/estadisticas.xlsx
+++ b/Documentos/estadisticas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="144" windowWidth="19620" windowHeight="9000"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="14340" windowHeight="7836"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="12">
   <si>
     <t>Bap: nveces</t>
   </si>
@@ -46,6 +47,12 @@
   </si>
   <si>
     <t>BVNS</t>
+  </si>
+  <si>
+    <t>Tabú</t>
+  </si>
+  <si>
+    <t>Busqueda Dispersa</t>
   </si>
 </sst>
 </file>
@@ -386,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:J91"/>
+    <sheetView tabSelected="1" topLeftCell="H28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -399,9 +406,10 @@
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +440,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -464,8 +478,14 @@
       <c r="J2" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="1">
+        <v>4</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -496,8 +516,14 @@
       <c r="J3" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="1">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -528,8 +554,14 @@
       <c r="J4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -560,8 +592,14 @@
       <c r="J5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="1">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -592,8 +630,14 @@
       <c r="J6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="1">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -624,8 +668,14 @@
       <c r="J7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="1">
+        <v>4</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -656,8 +706,14 @@
       <c r="J8" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="1">
+        <v>4</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -688,8 +744,14 @@
       <c r="J9" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="1">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -720,8 +782,14 @@
       <c r="J10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="1">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -752,8 +820,14 @@
       <c r="J11" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K11" s="1">
+        <v>4</v>
+      </c>
+      <c r="L11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,8 +858,14 @@
       <c r="J19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>10</v>
       </c>
@@ -816,8 +896,14 @@
       <c r="J20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>10</v>
       </c>
@@ -848,8 +934,14 @@
       <c r="J21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>10</v>
       </c>
@@ -880,8 +972,14 @@
       <c r="J22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>10</v>
+      </c>
+      <c r="L22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>10</v>
       </c>
@@ -912,8 +1010,14 @@
       <c r="J23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>11</v>
+      </c>
+      <c r="L23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>10</v>
       </c>
@@ -944,8 +1048,14 @@
       <c r="J24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>10</v>
+      </c>
+      <c r="L24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>10</v>
       </c>
@@ -976,8 +1086,14 @@
       <c r="J25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>10</v>
+      </c>
+      <c r="L25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>10</v>
       </c>
@@ -1008,8 +1124,14 @@
       <c r="J26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <v>10</v>
+      </c>
+      <c r="L26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1040,8 +1162,14 @@
       <c r="J27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <v>10</v>
+      </c>
+      <c r="L27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1072,8 +1200,14 @@
       <c r="J28">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28">
+        <v>12</v>
+      </c>
+      <c r="L28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1104,8 +1238,14 @@
       <c r="J29">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29">
+        <v>10</v>
+      </c>
+      <c r="L29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1136,8 +1276,14 @@
       <c r="J30">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K30">
+        <v>10</v>
+      </c>
+      <c r="L30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -1168,8 +1314,14 @@
       <c r="J40" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>37</v>
       </c>
@@ -1201,7 +1353,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>38</v>
       </c>
@@ -1233,7 +1385,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>38</v>
       </c>
@@ -1265,7 +1417,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>38</v>
       </c>
@@ -1297,7 +1449,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>37</v>
       </c>
@@ -1329,7 +1481,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>38</v>
       </c>
@@ -1361,7 +1513,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>38</v>
       </c>
@@ -1393,7 +1545,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>38</v>
       </c>
@@ -1425,7 +1577,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>37</v>
       </c>
@@ -1457,7 +1609,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>37</v>
       </c>
@@ -1489,7 +1641,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>38</v>
       </c>
@@ -1521,7 +1673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
@@ -1552,8 +1704,14 @@
       <c r="J60" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="K60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61">
         <v>12</v>
       </c>
@@ -1585,7 +1743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:12">
       <c r="A62">
         <v>12</v>
       </c>
@@ -1617,7 +1775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:12">
       <c r="A63">
         <v>12</v>
       </c>
@@ -1649,7 +1807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:12">
       <c r="A64">
         <v>12</v>
       </c>
@@ -1681,7 +1839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:12">
       <c r="A65">
         <v>12</v>
       </c>
@@ -1713,7 +1871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:12">
       <c r="A66">
         <v>12</v>
       </c>
@@ -1745,7 +1903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:12">
       <c r="A67">
         <v>12</v>
       </c>
@@ -1777,7 +1935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:12">
       <c r="A68">
         <v>12</v>
       </c>
@@ -1809,7 +1967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:12">
       <c r="A69">
         <v>12</v>
       </c>
@@ -1841,7 +1999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:12">
       <c r="A70">
         <v>12</v>
       </c>
@@ -1873,7 +2031,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:12">
       <c r="A71">
         <v>12</v>
       </c>
@@ -1905,7 +2063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:12">
       <c r="A80" s="1" t="s">
         <v>0</v>
       </c>
@@ -1936,6 +2094,12 @@
       <c r="J80" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K80" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81">
@@ -2287,6 +2451,41 @@
       </c>
       <c r="J91">
         <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12">
+      <c r="B97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>